<commit_message>
Added 2kr mean response time
</commit_message>
<xml_diff>
--- a/excel/verification/binomialVerification.xlsx
+++ b/excel/verification/binomialVerification.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t xml:space="preserve">95% CI</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t xml:space="preserve">Scatterplot samples vs normal calculated with the binomial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean</t>
   </si>
 </sst>
 </file>
@@ -274,7 +277,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -323,6 +326,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,8 +349,8 @@
   </sheetPr>
   <dimension ref="B1:BW209"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U7" activeCellId="0" sqref="U7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z2" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AJ47" activeCellId="0" sqref="AJ47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6280,6 +6287,121 @@
         <f aca="false">POWER(B47-$C$3, 2)/($F$3-1)</f>
         <v>2.32765511237734E-006</v>
       </c>
+      <c r="L47" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="M47" s="12" t="n">
+        <f aca="false">AVERAGE(M7:M46)</f>
+        <v>0.0950138888888889</v>
+      </c>
+      <c r="N47" s="12" t="n">
+        <f aca="false">AVERAGE(N7:N46)</f>
+        <v>0.178013888888889</v>
+      </c>
+      <c r="O47" s="12" t="n">
+        <f aca="false">AVERAGE(O7:O46)</f>
+        <v>0.254486111111111</v>
+      </c>
+      <c r="P47" s="12" t="n">
+        <f aca="false">AVERAGE(P7:P46)</f>
+        <v>0.318430555555556</v>
+      </c>
+      <c r="Q47" s="12" t="n">
+        <f aca="false">AVERAGE(Q7:Q46)</f>
+        <v>0.478972222222222</v>
+      </c>
+      <c r="R47" s="12" t="n">
+        <f aca="false">AVERAGE(R7:R46)</f>
+        <v>0.482708333333333</v>
+      </c>
+      <c r="S47" s="12" t="n">
+        <f aca="false">AVERAGE(S7:S46)</f>
+        <v>0.319958333333333</v>
+      </c>
+      <c r="T47" s="12" t="n">
+        <f aca="false">AVERAGE(T7:T46)</f>
+        <v>0.200319444444444</v>
+      </c>
+      <c r="U47" s="12" t="n">
+        <f aca="false">AVERAGE(U7:U46)</f>
+        <v>0.326972222222222</v>
+      </c>
+      <c r="V47" s="12" t="n">
+        <f aca="false">AVERAGE(V7:V46)</f>
+        <v>0.391736111111111</v>
+      </c>
+      <c r="W47" s="12" t="n">
+        <f aca="false">AVERAGE(W7:W46)</f>
+        <v>0.410291666666666</v>
+      </c>
+      <c r="X47" s="12" t="n">
+        <f aca="false">AVERAGE(X7:X46)</f>
+        <v>0.26075</v>
+      </c>
+      <c r="Y47" s="12" t="n">
+        <f aca="false">AVERAGE(Y7:Y46)</f>
+        <v>0.0781388888888888</v>
+      </c>
+      <c r="Z47" s="12" t="n">
+        <f aca="false">AVERAGE(Z7:Z46)</f>
+        <v>0.00654166666666666</v>
+      </c>
+      <c r="AA47" s="12" t="n">
+        <f aca="false">AVERAGE(AA7:AA46)</f>
+        <v>0.314458333333333</v>
+      </c>
+      <c r="AB47" s="12" t="n">
+        <f aca="false">AVERAGE(AB7:AB46)</f>
+        <v>0.386180555555555</v>
+      </c>
+      <c r="AC47" s="12" t="n">
+        <f aca="false">AVERAGE(AC7:AC46)</f>
+        <v>0.349277777777777</v>
+      </c>
+      <c r="AD47" s="12" t="n">
+        <f aca="false">AVERAGE(AD7:AD46)</f>
+        <v>0.270958333333333</v>
+      </c>
+      <c r="AE47" s="12" t="n">
+        <f aca="false">AVERAGE(AE7:AE46)</f>
+        <v>0.04</v>
+      </c>
+      <c r="AF47" s="12" t="n">
+        <f aca="false">AVERAGE(AF7:AF46)</f>
+        <v>0.00141666666666667</v>
+      </c>
+      <c r="AG47" s="12" t="n">
+        <f aca="false">AVERAGE(AG7:AG46)</f>
+        <v>0</v>
+      </c>
+      <c r="AH47" s="12" t="n">
+        <f aca="false">AVERAGE(AH7:AH46)</f>
+        <v>0.340861111111111</v>
+      </c>
+      <c r="AI47" s="12" t="n">
+        <f aca="false">AVERAGE(AI7:AI46)</f>
+        <v>0.141319444444445</v>
+      </c>
+      <c r="AJ47" s="12" t="n">
+        <f aca="false">AVERAGE(AJ7:AJ46)</f>
+        <v>0.0411666666666666</v>
+      </c>
+      <c r="AK47" s="12" t="n">
+        <f aca="false">AVERAGE(AK7:AK46)</f>
+        <v>0.00952777777777779</v>
+      </c>
+      <c r="AL47" s="12" t="n">
+        <f aca="false">AVERAGE(AL7:AL46)</f>
+        <v>0</v>
+      </c>
+      <c r="AM47" s="12" t="n">
+        <f aca="false">AVERAGE(AM7:AM46)</f>
+        <v>0</v>
+      </c>
+      <c r="AN47" s="12" t="n">
+        <f aca="false">AVERAGE(AN7:AN46)</f>
+        <v>0</v>
+      </c>
       <c r="AP47" s="0" t="n">
         <v>369</v>
       </c>

</xml_diff>

<commit_message>
Added Plots of response time
</commit_message>
<xml_diff>
--- a/excel/verification/binomialVerification.xlsx
+++ b/excel/verification/binomialVerification.xlsx
@@ -277,7 +277,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -286,7 +286,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -326,10 +326,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,11 +345,11 @@
   </sheetPr>
   <dimension ref="B1:BW209"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z2" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AJ47" activeCellId="0" sqref="AJ47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.98"/>
@@ -6290,115 +6286,115 @@
       <c r="L47" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="M47" s="12" t="n">
+      <c r="M47" s="4" t="n">
         <f aca="false">AVERAGE(M7:M46)</f>
         <v>0.0950138888888889</v>
       </c>
-      <c r="N47" s="12" t="n">
+      <c r="N47" s="4" t="n">
         <f aca="false">AVERAGE(N7:N46)</f>
         <v>0.178013888888889</v>
       </c>
-      <c r="O47" s="12" t="n">
+      <c r="O47" s="4" t="n">
         <f aca="false">AVERAGE(O7:O46)</f>
         <v>0.254486111111111</v>
       </c>
-      <c r="P47" s="12" t="n">
+      <c r="P47" s="4" t="n">
         <f aca="false">AVERAGE(P7:P46)</f>
         <v>0.318430555555556</v>
       </c>
-      <c r="Q47" s="12" t="n">
+      <c r="Q47" s="4" t="n">
         <f aca="false">AVERAGE(Q7:Q46)</f>
         <v>0.478972222222222</v>
       </c>
-      <c r="R47" s="12" t="n">
+      <c r="R47" s="4" t="n">
         <f aca="false">AVERAGE(R7:R46)</f>
         <v>0.482708333333333</v>
       </c>
-      <c r="S47" s="12" t="n">
+      <c r="S47" s="4" t="n">
         <f aca="false">AVERAGE(S7:S46)</f>
         <v>0.319958333333333</v>
       </c>
-      <c r="T47" s="12" t="n">
+      <c r="T47" s="4" t="n">
         <f aca="false">AVERAGE(T7:T46)</f>
         <v>0.200319444444444</v>
       </c>
-      <c r="U47" s="12" t="n">
+      <c r="U47" s="4" t="n">
         <f aca="false">AVERAGE(U7:U46)</f>
         <v>0.326972222222222</v>
       </c>
-      <c r="V47" s="12" t="n">
+      <c r="V47" s="4" t="n">
         <f aca="false">AVERAGE(V7:V46)</f>
         <v>0.391736111111111</v>
       </c>
-      <c r="W47" s="12" t="n">
+      <c r="W47" s="4" t="n">
         <f aca="false">AVERAGE(W7:W46)</f>
         <v>0.410291666666666</v>
       </c>
-      <c r="X47" s="12" t="n">
+      <c r="X47" s="4" t="n">
         <f aca="false">AVERAGE(X7:X46)</f>
         <v>0.26075</v>
       </c>
-      <c r="Y47" s="12" t="n">
+      <c r="Y47" s="4" t="n">
         <f aca="false">AVERAGE(Y7:Y46)</f>
         <v>0.0781388888888888</v>
       </c>
-      <c r="Z47" s="12" t="n">
+      <c r="Z47" s="4" t="n">
         <f aca="false">AVERAGE(Z7:Z46)</f>
         <v>0.00654166666666666</v>
       </c>
-      <c r="AA47" s="12" t="n">
+      <c r="AA47" s="4" t="n">
         <f aca="false">AVERAGE(AA7:AA46)</f>
         <v>0.314458333333333</v>
       </c>
-      <c r="AB47" s="12" t="n">
+      <c r="AB47" s="4" t="n">
         <f aca="false">AVERAGE(AB7:AB46)</f>
         <v>0.386180555555555</v>
       </c>
-      <c r="AC47" s="12" t="n">
+      <c r="AC47" s="4" t="n">
         <f aca="false">AVERAGE(AC7:AC46)</f>
         <v>0.349277777777777</v>
       </c>
-      <c r="AD47" s="12" t="n">
+      <c r="AD47" s="4" t="n">
         <f aca="false">AVERAGE(AD7:AD46)</f>
         <v>0.270958333333333</v>
       </c>
-      <c r="AE47" s="12" t="n">
+      <c r="AE47" s="4" t="n">
         <f aca="false">AVERAGE(AE7:AE46)</f>
         <v>0.04</v>
       </c>
-      <c r="AF47" s="12" t="n">
+      <c r="AF47" s="4" t="n">
         <f aca="false">AVERAGE(AF7:AF46)</f>
         <v>0.00141666666666667</v>
       </c>
-      <c r="AG47" s="12" t="n">
+      <c r="AG47" s="4" t="n">
         <f aca="false">AVERAGE(AG7:AG46)</f>
         <v>0</v>
       </c>
-      <c r="AH47" s="12" t="n">
+      <c r="AH47" s="4" t="n">
         <f aca="false">AVERAGE(AH7:AH46)</f>
         <v>0.340861111111111</v>
       </c>
-      <c r="AI47" s="12" t="n">
+      <c r="AI47" s="4" t="n">
         <f aca="false">AVERAGE(AI7:AI46)</f>
         <v>0.141319444444445</v>
       </c>
-      <c r="AJ47" s="12" t="n">
+      <c r="AJ47" s="4" t="n">
         <f aca="false">AVERAGE(AJ7:AJ46)</f>
         <v>0.0411666666666666</v>
       </c>
-      <c r="AK47" s="12" t="n">
+      <c r="AK47" s="4" t="n">
         <f aca="false">AVERAGE(AK7:AK46)</f>
         <v>0.00952777777777779</v>
       </c>
-      <c r="AL47" s="12" t="n">
+      <c r="AL47" s="4" t="n">
         <f aca="false">AVERAGE(AL7:AL46)</f>
         <v>0</v>
       </c>
-      <c r="AM47" s="12" t="n">
+      <c r="AM47" s="4" t="n">
         <f aca="false">AVERAGE(AM7:AM46)</f>
         <v>0</v>
       </c>
-      <c r="AN47" s="12" t="n">
+      <c r="AN47" s="4" t="n">
         <f aca="false">AVERAGE(AN7:AN46)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Aggiunto dati in caso response time non limitato alla doc
</commit_message>
<xml_diff>
--- a/excel/verification/binomialVerification.xlsx
+++ b/excel/verification/binomialVerification.xlsx
@@ -345,11 +345,11 @@
   </sheetPr>
   <dimension ref="B1:BW209"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AJ47" activeCellId="0" sqref="AJ47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="29" zoomScaleNormal="29" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S190" activeCellId="0" sqref="S190"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.98"/>

</xml_diff>

<commit_message>
Little correction on doc, changed a plot of binomial verification, underlined things that maybe we can delete
</commit_message>
<xml_diff>
--- a/excel/verification/binomialVerification.xlsx
+++ b/excel/verification/binomialVerification.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t xml:space="preserve">95% CI</t>
   </si>
@@ -135,6 +135,15 @@
   <si>
     <t xml:space="preserve">mean</t>
   </si>
+  <si>
+    <t xml:space="preserve">Simulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theoretical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N </t>
+  </si>
 </sst>
 </file>
 
@@ -144,7 +153,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -178,6 +187,26 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -335,7 +364,569 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF2A6099"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF8000"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1500" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1500" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Mean Throughput (Binomial Verification)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>binomialVerification!$AZ$81:$AZ$81</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Simulation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="ff8000">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff8000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="6"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="ff8000"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>binomialVerification!$AY$83:$AY$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>binomialVerification!$AZ$83:$AZ$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>355.61</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>717.77</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>897.51</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1079.68</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1437.59</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>binomialVerification!$BA$81</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Theoretical</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="2a6099"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="2a6099"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="2a6099"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>binomialVerification!$AY$82:$AY$88</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>binomialVerification!$BA$82:$BA$88</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1080</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1440</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="57772372"/>
+        <c:axId val="49298495"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="57772372"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>p</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1200" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="49298495"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="49298495"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Mean Throughput [packets/slot]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1100" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="57772372"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>106560</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>48960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>972000</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>59760</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="41503320" y="15004440"/>
+        <a:ext cx="7886520" cy="4562280"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -345,11 +936,11 @@
   </sheetPr>
   <dimension ref="B1:BW209"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="29" zoomScaleNormal="29" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S190" activeCellId="0" sqref="S190"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AS76" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BC87" activeCellId="0" sqref="BC87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.98"/>
@@ -7943,6 +8534,15 @@
       <c r="AT81" s="0" t="n">
         <v>907</v>
       </c>
+      <c r="AY81" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="AZ81" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="BA81" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="BF81" s="0" t="n">
         <v>881</v>
       </c>
@@ -7988,6 +8588,15 @@
       <c r="AT82" s="0" t="n">
         <v>881</v>
       </c>
+      <c r="AX82" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="AY82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA82" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="BF82" s="0" t="n">
         <v>898</v>
       </c>
@@ -8033,6 +8642,19 @@
       <c r="AT83" s="0" t="n">
         <v>898</v>
       </c>
+      <c r="AX83" s="0" t="n">
+        <v>1800</v>
+      </c>
+      <c r="AY83" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AZ83" s="0" t="n">
+        <v>355.61</v>
+      </c>
+      <c r="BA83" s="0" t="n">
+        <f aca="false">$AX$83*AY83</f>
+        <v>360</v>
+      </c>
       <c r="BF83" s="0" t="n">
         <v>919</v>
       </c>
@@ -8078,6 +8700,16 @@
       <c r="AT84" s="0" t="n">
         <v>919</v>
       </c>
+      <c r="AY84" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AZ84" s="0" t="n">
+        <v>717.77</v>
+      </c>
+      <c r="BA84" s="0" t="n">
+        <f aca="false">$AX$83*AY84</f>
+        <v>720</v>
+      </c>
       <c r="BF84" s="0" t="n">
         <v>902</v>
       </c>
@@ -8123,6 +8755,16 @@
       <c r="AT85" s="0" t="n">
         <v>902</v>
       </c>
+      <c r="AY85" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AZ85" s="0" t="n">
+        <v>897.51</v>
+      </c>
+      <c r="BA85" s="0" t="n">
+        <f aca="false">$AX$83*AY85</f>
+        <v>900</v>
+      </c>
       <c r="BF85" s="0" t="n">
         <v>923</v>
       </c>
@@ -8168,6 +8810,16 @@
       <c r="AT86" s="0" t="n">
         <v>923</v>
       </c>
+      <c r="AY86" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AZ86" s="0" t="n">
+        <v>1079.68</v>
+      </c>
+      <c r="BA86" s="0" t="n">
+        <f aca="false">$AX$83*AY86</f>
+        <v>1080</v>
+      </c>
       <c r="BF86" s="0" t="n">
         <v>937</v>
       </c>
@@ -8213,6 +8865,16 @@
       <c r="AT87" s="0" t="n">
         <v>937</v>
       </c>
+      <c r="AY87" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AZ87" s="0" t="n">
+        <v>1437.59</v>
+      </c>
+      <c r="BA87" s="0" t="n">
+        <f aca="false">$AX$83*AY87</f>
+        <v>1440</v>
+      </c>
       <c r="BF87" s="0" t="n">
         <v>931</v>
       </c>
@@ -8258,6 +8920,12 @@
       <c r="AT88" s="0" t="n">
         <v>931</v>
       </c>
+      <c r="AY88" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA88" s="0" t="n">
+        <v>1800</v>
+      </c>
       <c r="BF88" s="0" t="n">
         <v>894</v>
       </c>
@@ -8896,6 +9564,28 @@
       </c>
       <c r="BW102" s="0" t="n">
         <v>2.5758293035489</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP103" s="0" t="n">
+        <f aca="false">AVERAGE(AP3:AP102)</f>
+        <v>355.61</v>
+      </c>
+      <c r="AQ103" s="0" t="n">
+        <f aca="false">AVERAGE(AQ3:AQ102)</f>
+        <v>717.77</v>
+      </c>
+      <c r="AR103" s="0" t="n">
+        <f aca="false">AVERAGE(AR3:AR102)</f>
+        <v>1079.68</v>
+      </c>
+      <c r="AS103" s="0" t="n">
+        <f aca="false">AVERAGE(AS3:AS102)</f>
+        <v>1437.59</v>
+      </c>
+      <c r="AT103" s="0" t="n">
+        <f aca="false">AVERAGE(AT3:AT102)</f>
+        <v>897.51</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9413,5 +10103,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>